<commit_message>
update from a new build to add new modules
</commit_message>
<xml_diff>
--- a/t/data/R8949_999999999_2019.xlsx
+++ b/t/data/R8949_999999999_2019.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Form 8939 Report'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Form 8939 Report'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Form 8939 Report'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Form 8939 Report'!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="47">
   <si>
     <t xml:space="preserve">Ignore</t>
   </si>
@@ -75,7 +76,7 @@
     <t xml:space="preserve">UserBasis</t>
   </si>
   <si>
-    <t xml:space="preserve">UserCode</t>
+    <t xml:space="preserve">UserCodes</t>
   </si>
   <si>
     <t xml:space="preserve">y</t>
@@ -97,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">boxA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">SELECTED AMERN SHS INC CL S (SLASX)</t>
@@ -287,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,10 +354,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -488,9 +488,9 @@
   <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B75" activeCellId="0" sqref="B75:O78"/>
+      <selection pane="bottomLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,8 +499,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="8.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="4.57"/>
@@ -564,7 +564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -585,40 +585,38 @@
       <c r="N2" s="13"/>
       <c r="O2" s="15"/>
     </row>
-    <row r="3" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-    </row>
-    <row r="4" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>43630</v>
       </c>
-      <c r="F4" s="4"/>
       <c r="G4" s="4" t="n">
         <v>43452</v>
       </c>
@@ -631,8 +629,6 @@
       <c r="J4" s="6" t="n">
         <v>1422.42</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
       <c r="M4" s="2" t="s">
         <v>22</v>
       </c>
@@ -642,20 +638,24 @@
       <c r="O4" s="6" t="n">
         <v>290.55</v>
       </c>
-    </row>
-    <row r="5" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F5" s="4"/>
       <c r="G5" s="4" t="n">
         <v>43452</v>
       </c>
@@ -668,8 +668,6 @@
       <c r="J5" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
       <c r="M5" s="2" t="s">
         <v>22</v>
       </c>
@@ -680,19 +678,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="6" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F6" s="4"/>
       <c r="G6" s="4" t="n">
         <v>43452</v>
       </c>
@@ -705,8 +701,6 @@
       <c r="J6" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
       <c r="M6" s="2" t="s">
         <v>22</v>
       </c>
@@ -717,19 +711,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="7" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F7" s="4"/>
       <c r="G7" s="4" t="n">
         <v>43452</v>
       </c>
@@ -742,8 +734,6 @@
       <c r="J7" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
       <c r="M7" s="2" t="s">
         <v>22</v>
       </c>
@@ -754,19 +744,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="8" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F8" s="4"/>
       <c r="G8" s="4" t="n">
         <v>43452</v>
       </c>
@@ -779,8 +767,6 @@
       <c r="J8" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
       <c r="M8" s="2" t="s">
         <v>22</v>
       </c>
@@ -791,19 +777,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="9" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F9" s="4"/>
       <c r="G9" s="4" t="n">
         <v>43452</v>
       </c>
@@ -816,8 +800,6 @@
       <c r="J9" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
       <c r="M9" s="2" t="s">
         <v>22</v>
       </c>
@@ -828,19 +810,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="10" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F10" s="4"/>
       <c r="G10" s="4" t="n">
         <v>43452</v>
       </c>
@@ -853,8 +833,6 @@
       <c r="J10" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
       <c r="M10" s="2" t="s">
         <v>22</v>
       </c>
@@ -865,19 +843,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="11" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
       <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4" t="n">
         <v>43452</v>
       </c>
@@ -890,8 +866,6 @@
       <c r="J11" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
       <c r="M11" s="2" t="s">
         <v>22</v>
       </c>
@@ -902,19 +876,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="12" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F12" s="4"/>
       <c r="G12" s="4" t="n">
         <v>43452</v>
       </c>
@@ -927,8 +899,6 @@
       <c r="J12" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
       <c r="M12" s="2" t="s">
         <v>22</v>
       </c>
@@ -939,19 +909,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="13" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F13" s="4"/>
       <c r="G13" s="4" t="n">
         <v>43452</v>
       </c>
@@ -964,8 +932,6 @@
       <c r="J13" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
       <c r="M13" s="2" t="s">
         <v>22</v>
       </c>
@@ -976,19 +942,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="14" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F14" s="4"/>
       <c r="G14" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1001,8 +965,6 @@
       <c r="J14" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
       <c r="M14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1013,19 +975,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="15" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="G15" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1038,8 +998,6 @@
       <c r="J15" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
       <c r="M15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1050,19 +1008,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="16" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F16" s="4"/>
       <c r="G16" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1075,8 +1031,6 @@
       <c r="J16" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
       <c r="M16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1087,19 +1041,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="17" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F17" s="4"/>
       <c r="G17" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1112,8 +1064,6 @@
       <c r="J17" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
       <c r="M17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1124,19 +1074,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="18" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F18" s="4"/>
       <c r="G18" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1149,8 +1097,6 @@
       <c r="J18" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
       <c r="M18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1161,19 +1107,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="19" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
       <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>25</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F19" s="4"/>
       <c r="G19" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1186,8 +1130,6 @@
       <c r="J19" s="6" t="n">
         <v>3168.64</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
       <c r="M19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1198,19 +1140,17 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="20" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>27</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F20" s="4"/>
       <c r="G20" s="4" t="n">
         <v>43452</v>
       </c>
@@ -1223,8 +1163,6 @@
       <c r="J20" s="6" t="n">
         <v>1706.4</v>
       </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
       <c r="M20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1235,40 +1173,38 @@
         <v>123.57</v>
       </c>
     </row>
-    <row r="21" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-    </row>
-    <row r="22" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F22" s="4"/>
       <c r="G22" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1281,31 +1217,27 @@
       <c r="J22" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
       <c r="M22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O22" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="23" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F23" s="4"/>
       <c r="G23" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1318,31 +1250,27 @@
       <c r="J23" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
       <c r="M23" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O23" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="24" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D24" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F24" s="4"/>
       <c r="G24" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1355,31 +1283,27 @@
       <c r="J24" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
       <c r="M24" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O24" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="25" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F25" s="4"/>
       <c r="G25" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1392,31 +1316,27 @@
       <c r="J25" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
       <c r="M25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O25" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="26" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F26" s="4"/>
       <c r="G26" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1429,31 +1349,27 @@
       <c r="J26" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
       <c r="M26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O26" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="27" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
       <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F27" s="4"/>
       <c r="G27" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1466,31 +1382,27 @@
       <c r="J27" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
       <c r="M27" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O27" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="28" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
       <c r="B28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F28" s="4"/>
       <c r="G28" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1503,31 +1415,27 @@
       <c r="J28" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
       <c r="M28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O28" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="29" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D29" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F29" s="4"/>
       <c r="G29" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1540,31 +1448,27 @@
       <c r="J29" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
       <c r="M29" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O29" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="30" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F30" s="4"/>
       <c r="G30" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1577,31 +1481,27 @@
       <c r="J30" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
       <c r="M30" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O30" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="31" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
       <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F31" s="4"/>
       <c r="G31" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1614,31 +1514,27 @@
       <c r="J31" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
       <c r="M31" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O31" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="32" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
       <c r="B32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D32" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F32" s="4"/>
       <c r="G32" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1651,31 +1547,27 @@
       <c r="J32" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
       <c r="M32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O32" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="33" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
       <c r="B33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F33" s="4"/>
       <c r="G33" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1688,31 +1580,27 @@
       <c r="J33" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
       <c r="M33" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O33" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="34" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
       <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D34" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F34" s="4"/>
       <c r="G34" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1725,31 +1613,27 @@
       <c r="J34" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
       <c r="M34" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O34" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="35" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
       <c r="B35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D35" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E35" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F35" s="4"/>
       <c r="G35" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1762,31 +1646,27 @@
       <c r="J35" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
       <c r="M35" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O35" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="36" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
       <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F36" s="4"/>
       <c r="G36" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1799,31 +1679,27 @@
       <c r="J36" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
       <c r="M36" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O36" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="37" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
       <c r="B37" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D37" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F37" s="4"/>
       <c r="G37" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1836,31 +1712,27 @@
       <c r="J37" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
       <c r="M37" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O37" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="38" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
       <c r="B38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>30</v>
+      </c>
       <c r="D38" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>43670</v>
       </c>
-      <c r="F38" s="4"/>
       <c r="G38" s="4" t="n">
         <v>37517</v>
       </c>
@@ -1873,73 +1745,69 @@
       <c r="J38" s="6" t="n">
         <v>2551.48</v>
       </c>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
       <c r="M38" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O38" s="6" t="n">
         <v>97.6</v>
       </c>
     </row>
-    <row r="39" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="24"/>
-    </row>
-    <row r="40" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="23"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="29"/>
-    </row>
-    <row r="41" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="28"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11"/>
       <c r="B41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D41" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F41" s="4"/>
       <c r="G41" s="4" t="n">
         <v>43542</v>
       </c>
@@ -1952,31 +1820,27 @@
       <c r="J41" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
       <c r="M41" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O41" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="42" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11"/>
       <c r="B42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F42" s="4"/>
       <c r="G42" s="4" t="n">
         <v>43542</v>
       </c>
@@ -1989,31 +1853,27 @@
       <c r="J42" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
       <c r="M42" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O42" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="43" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11"/>
       <c r="B43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F43" s="4"/>
       <c r="G43" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2026,31 +1886,27 @@
       <c r="J43" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
       <c r="M43" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O43" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="44" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11"/>
       <c r="B44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D44" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F44" s="4"/>
       <c r="G44" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2063,31 +1919,27 @@
       <c r="J44" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
       <c r="M44" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O44" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="45" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11"/>
       <c r="B45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D45" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F45" s="4"/>
       <c r="G45" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2100,31 +1952,27 @@
       <c r="J45" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
       <c r="M45" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O45" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="46" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11"/>
       <c r="B46" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D46" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E46" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F46" s="4"/>
       <c r="G46" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2137,31 +1985,27 @@
       <c r="J46" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
       <c r="M46" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O46" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="47" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11"/>
       <c r="B47" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D47" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E47" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F47" s="4"/>
       <c r="G47" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2174,31 +2018,27 @@
       <c r="J47" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
       <c r="M47" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O47" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="48" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11"/>
       <c r="B48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D48" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E48" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F48" s="4"/>
       <c r="G48" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2211,31 +2051,27 @@
       <c r="J48" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
       <c r="M48" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O48" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="49" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11"/>
       <c r="B49" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D49" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E49" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F49" s="4"/>
       <c r="G49" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2248,31 +2084,27 @@
       <c r="J49" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
       <c r="M49" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O49" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="50" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11"/>
       <c r="B50" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D50" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E50" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F50" s="4"/>
       <c r="G50" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2285,31 +2117,27 @@
       <c r="J50" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
       <c r="M50" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O50" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="51" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11"/>
       <c r="B51" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E51" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F51" s="4"/>
       <c r="G51" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2322,31 +2150,27 @@
       <c r="J51" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
       <c r="M51" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O51" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="52" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E52" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F52" s="4"/>
       <c r="G52" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2359,31 +2183,27 @@
       <c r="J52" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
       <c r="M52" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O52" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="53" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11"/>
       <c r="B53" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E53" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F53" s="4"/>
       <c r="G53" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2396,31 +2216,27 @@
       <c r="J53" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
       <c r="M53" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O53" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="54" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11"/>
       <c r="B54" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D54" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E54" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F54" s="4"/>
       <c r="G54" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2433,31 +2249,27 @@
       <c r="J54" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
       <c r="M54" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O54" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="55" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11"/>
       <c r="B55" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D55" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E55" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F55" s="4"/>
       <c r="G55" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2470,31 +2282,27 @@
       <c r="J55" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
       <c r="M55" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O55" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="56" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11"/>
       <c r="B56" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D56" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E56" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F56" s="4"/>
       <c r="G56" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2507,31 +2315,27 @@
       <c r="J56" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
       <c r="M56" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O56" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="57" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11"/>
       <c r="B57" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="2"/>
+        <v>36</v>
+      </c>
       <c r="D57" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E57" s="3" t="n">
         <v>43620</v>
       </c>
-      <c r="F57" s="4"/>
       <c r="G57" s="4" t="n">
         <v>43542</v>
       </c>
@@ -2544,45 +2348,43 @@
       <c r="J57" s="6" t="n">
         <v>6004.61</v>
       </c>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
       <c r="M57" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O57" s="6" t="n">
         <v>-445.2</v>
       </c>
     </row>
-    <row r="58" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="29"/>
+      <c r="B58" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="28"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E59" s="3" t="n">
         <v>43620</v>
@@ -2600,10 +2402,10 @@
         <v>6004.61</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O59" s="6" t="n">
         <v>-445.2</v>
@@ -2611,10 +2413,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E60" s="3" t="n">
         <v>43620</v>
@@ -2632,10 +2434,10 @@
         <v>2258.75</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O60" s="6" t="n">
         <v>-814.22</v>
@@ -2643,10 +2445,10 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E61" s="3" t="n">
         <v>43620</v>
@@ -2664,10 +2466,10 @@
         <v>4774.5</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O61" s="6" t="n">
         <v>1419.41</v>
@@ -2675,10 +2477,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E62" s="3" t="n">
         <v>43620</v>
@@ -2696,10 +2498,10 @@
         <v>4653.22</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O62" s="6" t="n">
         <v>-209.45</v>
@@ -2707,10 +2509,10 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E63" s="3" t="n">
         <v>43620</v>
@@ -2728,10 +2530,10 @@
         <v>6004.61</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O63" s="6" t="n">
         <v>-445.2</v>
@@ -2739,10 +2541,10 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E64" s="3" t="n">
         <v>43620</v>
@@ -2760,10 +2562,10 @@
         <v>2258.75</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O64" s="6" t="n">
         <v>-814.22</v>
@@ -2771,10 +2573,10 @@
     </row>
     <row r="65" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E65" s="3" t="n">
         <v>43620</v>
@@ -2792,10 +2594,10 @@
         <v>4774.5</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O65" s="6" t="n">
         <v>1419.41</v>
@@ -2803,10 +2605,10 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E66" s="3" t="n">
         <v>43620</v>
@@ -2824,10 +2626,10 @@
         <v>4653.22</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O66" s="6" t="n">
         <v>-209.45</v>
@@ -2835,10 +2637,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>43620</v>
@@ -2856,10 +2658,10 @@
         <v>6004.61</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O67" s="6" t="n">
         <v>-445.2</v>
@@ -2867,10 +2669,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E68" s="3" t="n">
         <v>43620</v>
@@ -2888,10 +2690,10 @@
         <v>2258.75</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O68" s="6" t="n">
         <v>-814.22</v>
@@ -2899,10 +2701,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E69" s="3" t="n">
         <v>43620</v>
@@ -2920,10 +2722,10 @@
         <v>4774.5</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O69" s="6" t="n">
         <v>1419.41</v>
@@ -2931,10 +2733,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E70" s="3" t="n">
         <v>43620</v>
@@ -2952,10 +2754,10 @@
         <v>4653.22</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O70" s="6" t="n">
         <v>-209.45</v>
@@ -2963,10 +2765,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E71" s="3" t="n">
         <v>43620</v>
@@ -2984,10 +2786,10 @@
         <v>6004.61</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O71" s="6" t="n">
         <v>-445.2</v>
@@ -2995,10 +2797,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E72" s="3" t="n">
         <v>43620</v>
@@ -3016,10 +2818,10 @@
         <v>2258.75</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O72" s="6" t="n">
         <v>-814.22</v>
@@ -3027,10 +2829,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E73" s="3" t="n">
         <v>43620</v>
@@ -3048,10 +2850,10 @@
         <v>4774.5</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O73" s="6" t="n">
         <v>1419.41</v>
@@ -3059,10 +2861,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E74" s="3" t="n">
         <v>43620</v>
@@ -3080,10 +2882,10 @@
         <v>4653.22</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O74" s="6" t="n">
         <v>-209.45</v>
@@ -3091,10 +2893,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E75" s="3" t="n">
         <v>43620</v>
@@ -3112,10 +2914,10 @@
         <v>6004.61</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O75" s="6" t="n">
         <v>-445.2</v>
@@ -3123,10 +2925,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E76" s="3" t="n">
         <v>43620</v>
@@ -3144,10 +2946,10 @@
         <v>2258.75</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O76" s="6" t="n">
         <v>-814.22</v>
@@ -3155,10 +2957,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E77" s="3" t="n">
         <v>43620</v>
@@ -3176,10 +2978,10 @@
         <v>4774.5</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O77" s="6" t="n">
         <v>1419.41</v>
@@ -3187,10 +2989,10 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E78" s="3" t="n">
         <v>43620</v>
@@ -3208,10 +3010,10 @@
         <v>4653.22</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O78" s="6" t="n">
         <v>-209.45</v>

</xml_diff>